<commit_message>
Added FP of new usecases
</commit_message>
<xml_diff>
--- a/documentation/UC time spent.xlsx
+++ b/documentation/UC time spent.xlsx
@@ -1,31 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10410"/>
-  <workbookPr defaultThemeVersion="166925"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/d0272129/OneDrive - dm drogerie/4. Semester/SE/"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{71F8A757-FF29-3B41-9161-5D8FC0491C63}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="9302"/>
+  <workbookPr/>
   <bookViews>
-    <workbookView xWindow="380" yWindow="440" windowWidth="28040" windowHeight="16400" xr2:uid="{9316D68E-33E7-DB46-AB0B-0A279E2DCD34}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" activeTab="0"/>
   </bookViews>
   <sheets>
-    <sheet name="Blatt1" sheetId="1" r:id="rId1"/>
+    <sheet name="Blatt1" sheetId="1" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="162913"/>
-  <extLst>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
-      <x15:workbookPr chartTrackingRefBase="1"/>
-    </ext>
-  </extLst>
+  <definedNames/>
+  <calcPr fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="27">
   <si>
     <t>UC </t>
   </si>
@@ -82,34 +72,71 @@
   </si>
   <si>
     <t>Refactoring</t>
+  </si>
+  <si>
+    <t>NEW Ucs</t>
+  </si>
+  <si>
+    <t>Discord</t>
+  </si>
+  <si>
+    <t>-</t>
+  </si>
+  <si>
+    <t>Notifications2</t>
+  </si>
+  <si>
+    <t>Tutorial</t>
+  </si>
+  <si>
+    <t>Signup2</t>
+  </si>
+  <si>
+    <t>Friends2</t>
+  </si>
+  <si>
+    <t>History2</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <numFmts count="2">
+    <numFmt numFmtId="164" formatCode="GENERAL"/>
+    <numFmt numFmtId="165" formatCode="GENERAL"/>
+  </numFmts>
+  <fonts count="4">
+    <font>
+      <sz val="10"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
     <font>
       <sz val="12"/>
-      <color theme="1"/>
+      <color indexed="8"/>
       <name val="Calibri"/>
       <family val="2"/>
-      <scheme val="minor"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="13"/>
-      <color rgb="FF444444"/>
+      <color indexed="63"/>
       <name val="Inherit"/>
+      <family val="0"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="13"/>
-      <color rgb="FFFF6600"/>
+      <color indexed="53"/>
       <name val="Inherit"/>
+      <family val="0"/>
+      <charset val="1"/>
     </font>
   </fonts>
   <fills count="2">
     <fill>
-      <patternFill patternType="none"/>
+      <patternFill/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
@@ -124,32 +151,134 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+  <cellStyleXfs count="21">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0">
+      <alignment/>
+      <protection/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="43" fontId="0" fillId="0" borderId="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="41" fontId="0" fillId="0" borderId="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="0">
+      <alignment/>
+      <protection/>
+    </xf>
   </cellStyleXfs>
-  <cellXfs count="3">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+  <cellXfs count="4">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment/>
+    </xf>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="20">
+      <alignment/>
+      <protection/>
+    </xf>
+    <xf numFmtId="164" fontId="2" fillId="0" borderId="0" xfId="20" applyFont="1" applyBorder="1">
+      <alignment/>
+      <protection/>
+    </xf>
+    <xf numFmtId="164" fontId="3" fillId="0" borderId="0" xfId="20" applyFont="1">
+      <alignment/>
+      <protection/>
+    </xf>
   </cellXfs>
-  <cellStyles count="1">
-    <cellStyle name="Standard" xfId="0" builtinId="0"/>
+  <cellStyles count="7">
+    <cellStyle name="Normal" xfId="0"/>
+    <cellStyle name="Comma" xfId="15"/>
+    <cellStyle name="Comma [0]" xfId="16"/>
+    <cellStyle name="Currency" xfId="17"/>
+    <cellStyle name="Currency [0]" xfId="18"/>
+    <cellStyle name="Percent" xfId="19"/>
+    <cellStyle name="Excel Built-in Normal" xfId="20"/>
   </cellStyles>
-  <dxfs count="0"/>
-  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
-      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
-      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
-    </ext>
-  </extLst>
+  <colors>
+    <indexedColors>
+      <rgbColor rgb="00000000"/>
+      <rgbColor rgb="00FFFFFF"/>
+      <rgbColor rgb="00FF0000"/>
+      <rgbColor rgb="0000FF00"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00000000"/>
+      <rgbColor rgb="00FFFFFF"/>
+      <rgbColor rgb="00FF0000"/>
+      <rgbColor rgb="0000FF00"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00800000"/>
+      <rgbColor rgb="00008000"/>
+      <rgbColor rgb="00000080"/>
+      <rgbColor rgb="00808000"/>
+      <rgbColor rgb="00800080"/>
+      <rgbColor rgb="00008080"/>
+      <rgbColor rgb="00C0C0C0"/>
+      <rgbColor rgb="00808080"/>
+      <rgbColor rgb="009999FF"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00FFFFCC"/>
+      <rgbColor rgb="00CCFFFF"/>
+      <rgbColor rgb="00660066"/>
+      <rgbColor rgb="00FF8080"/>
+      <rgbColor rgb="000066CC"/>
+      <rgbColor rgb="00CCCCFF"/>
+      <rgbColor rgb="00000080"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00800080"/>
+      <rgbColor rgb="00800000"/>
+      <rgbColor rgb="00008080"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="0000CCFF"/>
+      <rgbColor rgb="00CCFFFF"/>
+      <rgbColor rgb="00CCFFCC"/>
+      <rgbColor rgb="00FFFF99"/>
+      <rgbColor rgb="0099CCFF"/>
+      <rgbColor rgb="00FF99CC"/>
+      <rgbColor rgb="00CC99FF"/>
+      <rgbColor rgb="00FFCC99"/>
+      <rgbColor rgb="003366FF"/>
+      <rgbColor rgb="0033CCCC"/>
+      <rgbColor rgb="0099CC00"/>
+      <rgbColor rgb="00FFCC00"/>
+      <rgbColor rgb="00FF9900"/>
+      <rgbColor rgb="00FF6600"/>
+      <rgbColor rgb="00666699"/>
+      <rgbColor rgb="00969696"/>
+      <rgbColor rgb="00003366"/>
+      <rgbColor rgb="00339966"/>
+      <rgbColor rgb="00003300"/>
+      <rgbColor rgb="00333300"/>
+      <rgbColor rgb="00993300"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00333399"/>
+      <rgbColor rgb="00444444"/>
+    </indexedColors>
+  </colors>
 </styleSheet>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -444,24 +573,25 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{413A5E80-7608-814C-A553-C5BC4499381C}">
-  <dimension ref="A1:G13"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <dimension ref="A1:G22"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="E18" sqref="E18"/>
+    <sheetView tabSelected="1" workbookViewId="0" topLeftCell="A1">
+      <selection pane="topLeft" activeCell="G22" sqref="G22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
+  <sheetFormatPr defaultRowHeight="12.75"/>
   <cols>
-    <col min="1" max="1" width="28" customWidth="1"/>
-    <col min="2" max="2" width="14.5" customWidth="1"/>
-    <col min="3" max="3" width="7.5" customWidth="1"/>
-    <col min="4" max="4" width="8.1640625" customWidth="1"/>
-    <col min="5" max="5" width="52.5" customWidth="1"/>
-    <col min="6" max="6" width="6.5" customWidth="1"/>
+    <col min="1" max="1" width="30.7142857142857" style="1"/>
+    <col min="2" max="2" width="16" style="1"/>
+    <col min="3" max="3" width="8.28571428571429" style="1"/>
+    <col min="4" max="4" width="9" style="1"/>
+    <col min="5" max="5" width="57.7142857142857" style="1"/>
+    <col min="6" max="6" width="7.14285714285714" style="1"/>
+    <col min="7" max="16384" width="11.7142857142857" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="17" hidden="1">
+    <row r="1" spans="1:7" ht="12.75" hidden="1">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -474,7 +604,7 @@
       <c r="D1" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="E1" s="3" t="s">
         <v>4</v>
       </c>
       <c r="F1" s="2" t="s">
@@ -484,238 +614,382 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:7" ht="17">
+    <row r="2" spans="1:7" ht="12.75">
       <c r="A2" s="2"/>
       <c r="B2" s="2"/>
       <c r="C2" s="2"/>
       <c r="D2" s="2"/>
-      <c r="E2" s="1" t="s">
+      <c r="E2" s="3" t="s">
         <v>7</v>
       </c>
       <c r="F2" s="2"/>
       <c r="G2" s="2"/>
     </row>
-    <row r="3" spans="1:7">
-      <c r="A3" t="s">
+    <row r="3" spans="1:6" ht="12.75">
+      <c r="A3" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="B3">
+      <c r="B3" s="1">
         <v>2</v>
       </c>
-      <c r="C3">
+      <c r="C3" s="1">
         <v>9</v>
       </c>
-      <c r="D3">
-        <v>1</v>
-      </c>
-      <c r="E3">
-        <v>0</v>
-      </c>
-      <c r="F3">
+      <c r="D3" s="1">
+        <v>1</v>
+      </c>
+      <c r="E3" s="1">
+        <v>0</v>
+      </c>
+      <c r="F3" s="1">
         <v>12</v>
       </c>
     </row>
-    <row r="4" spans="1:7">
-      <c r="A4" t="s">
+    <row r="4" spans="1:6" ht="12.75">
+      <c r="A4" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="B4">
+      <c r="B4" s="1">
         <v>3</v>
       </c>
-      <c r="C4">
+      <c r="C4" s="1">
         <v>12</v>
       </c>
-      <c r="D4">
-        <v>1</v>
-      </c>
-      <c r="E4">
+      <c r="D4" s="1">
+        <v>1</v>
+      </c>
+      <c r="E4" s="1">
         <v>11</v>
       </c>
-      <c r="F4">
+      <c r="F4" s="1">
         <v>27</v>
       </c>
     </row>
-    <row r="5" spans="1:7">
-      <c r="A5" t="s">
+    <row r="5" spans="1:6" ht="12.75">
+      <c r="A5" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="B5">
-        <v>1</v>
-      </c>
-      <c r="C5">
+      <c r="B5" s="1">
+        <v>1</v>
+      </c>
+      <c r="C5" s="1">
         <v>4</v>
       </c>
-      <c r="D5">
-        <v>1</v>
-      </c>
-      <c r="E5">
-        <v>0</v>
-      </c>
-      <c r="F5">
+      <c r="D5" s="1">
+        <v>1</v>
+      </c>
+      <c r="E5" s="1">
+        <v>0</v>
+      </c>
+      <c r="F5" s="1">
         <v>6</v>
       </c>
     </row>
-    <row r="6" spans="1:7">
-      <c r="A6" t="s">
+    <row r="6" spans="1:6" ht="12.75">
+      <c r="A6" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="B6">
+      <c r="B6" s="1">
         <v>2</v>
       </c>
-      <c r="C6">
+      <c r="C6" s="1">
         <v>7</v>
       </c>
-      <c r="D6">
-        <v>1</v>
-      </c>
-      <c r="E6">
-        <v>1</v>
-      </c>
-      <c r="F6">
+      <c r="D6" s="1">
+        <v>1</v>
+      </c>
+      <c r="E6" s="1">
+        <v>1</v>
+      </c>
+      <c r="F6" s="1">
         <v>11</v>
       </c>
     </row>
-    <row r="7" spans="1:7">
-      <c r="A7" t="s">
+    <row r="7" spans="1:6" ht="12.75">
+      <c r="A7" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="B7">
-        <v>1</v>
-      </c>
-      <c r="C7">
+      <c r="B7" s="1">
+        <v>1</v>
+      </c>
+      <c r="C7" s="1">
         <v>3</v>
       </c>
-      <c r="D7">
-        <v>0</v>
-      </c>
-      <c r="E7">
-        <v>1</v>
-      </c>
-      <c r="F7">
+      <c r="D7" s="1">
+        <v>0</v>
+      </c>
+      <c r="E7" s="1">
+        <v>1</v>
+      </c>
+      <c r="F7" s="1">
         <v>5</v>
       </c>
     </row>
-    <row r="8" spans="1:7">
-      <c r="A8" t="s">
+    <row r="8" spans="1:6" ht="12.75">
+      <c r="A8" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="B8">
-        <v>1</v>
-      </c>
-      <c r="C8">
+      <c r="B8" s="1">
+        <v>1</v>
+      </c>
+      <c r="C8" s="1">
         <v>3</v>
       </c>
-      <c r="D8">
-        <v>1</v>
-      </c>
-      <c r="E8">
-        <v>0</v>
-      </c>
-      <c r="F8">
+      <c r="D8" s="1">
+        <v>1</v>
+      </c>
+      <c r="E8" s="1">
+        <v>0</v>
+      </c>
+      <c r="F8" s="1">
         <v>5</v>
       </c>
     </row>
-    <row r="9" spans="1:7">
-      <c r="A9" t="s">
+    <row r="9" spans="1:6" ht="12.75">
+      <c r="A9" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="B9">
-        <v>0</v>
-      </c>
-      <c r="C9">
-        <v>1</v>
-      </c>
-      <c r="D9">
-        <v>0</v>
-      </c>
-      <c r="E9">
-        <v>0</v>
-      </c>
-      <c r="F9">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="10" spans="1:7">
-      <c r="A10" t="s">
+      <c r="B9" s="1">
+        <v>0</v>
+      </c>
+      <c r="C9" s="1">
+        <v>1</v>
+      </c>
+      <c r="D9" s="1">
+        <v>0</v>
+      </c>
+      <c r="E9" s="1">
+        <v>0</v>
+      </c>
+      <c r="F9" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" ht="12.75">
+      <c r="A10" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="B10">
-        <v>0</v>
-      </c>
-      <c r="C10">
+      <c r="B10" s="1">
+        <v>0</v>
+      </c>
+      <c r="C10" s="1">
         <v>2</v>
       </c>
-      <c r="D10">
-        <v>0</v>
-      </c>
-      <c r="E10">
-        <v>0</v>
-      </c>
-      <c r="F10">
+      <c r="D10" s="1">
+        <v>0</v>
+      </c>
+      <c r="E10" s="1">
+        <v>0</v>
+      </c>
+      <c r="F10" s="1">
         <v>2</v>
       </c>
     </row>
-    <row r="11" spans="1:7">
-      <c r="A11" t="s">
+    <row r="11" spans="1:6" ht="12.75">
+      <c r="A11" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="B11">
+      <c r="B11" s="1">
         <v>12</v>
       </c>
-      <c r="C11">
-        <v>0</v>
-      </c>
-      <c r="D11">
-        <v>0</v>
-      </c>
-      <c r="E11">
-        <v>0</v>
-      </c>
-      <c r="F11">
+      <c r="C11" s="1">
+        <v>0</v>
+      </c>
+      <c r="D11" s="1">
+        <v>0</v>
+      </c>
+      <c r="E11" s="1">
+        <v>0</v>
+      </c>
+      <c r="F11" s="1">
         <v>12</v>
       </c>
     </row>
-    <row r="12" spans="1:7">
-      <c r="A12" t="s">
+    <row r="12" spans="1:6" ht="12.75">
+      <c r="A12" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="B12">
-        <v>0</v>
-      </c>
-      <c r="C12">
+      <c r="B12" s="1">
+        <v>0</v>
+      </c>
+      <c r="C12" s="1">
         <v>3</v>
       </c>
-      <c r="D12">
-        <v>1</v>
-      </c>
-      <c r="E12">
+      <c r="D12" s="1">
+        <v>1</v>
+      </c>
+      <c r="E12" s="1">
         <v>2</v>
       </c>
-      <c r="F12">
+      <c r="F12" s="1">
         <v>6</v>
       </c>
     </row>
-    <row r="13" spans="1:7">
-      <c r="A13" t="s">
+    <row r="13" spans="1:6" ht="12.75">
+      <c r="A13" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="B13">
-        <v>0</v>
-      </c>
-      <c r="C13">
+      <c r="B13" s="1">
+        <v>0</v>
+      </c>
+      <c r="C13" s="1">
         <v>18</v>
       </c>
-      <c r="D13">
-        <v>0</v>
-      </c>
-      <c r="E13">
+      <c r="D13" s="1">
+        <v>0</v>
+      </c>
+      <c r="E13" s="1">
         <v>2</v>
       </c>
-      <c r="F13">
+      <c r="F13" s="1">
         <v>20</v>
       </c>
     </row>
+    <row r="15" spans="1:1" ht="12.75">
+      <c r="A15" s="1" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" ht="12.75">
+      <c r="A17" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="B17" s="1">
+        <v>2</v>
+      </c>
+      <c r="C17" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="D17" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="E17" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="F17" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="G17" s="1">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" ht="12.75">
+      <c r="A18" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="B18" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="C18" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="D18" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="E18" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="F18" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="G18" s="1">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" ht="12.75">
+      <c r="A19" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="B19" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="C19" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="D19" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="E19" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="F19" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="G19" s="1">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" ht="12.75">
+      <c r="A20" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="B20" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="C20" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="D20" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="E20" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="F20" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="G20" s="1">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" ht="12.75">
+      <c r="A21" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="B21" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="C21" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="D21" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="E21" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="F21" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="G21" s="1">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" ht="12.75">
+      <c r="A22" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="B22" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="C22" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="D22" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="E22" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="F22" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="G22" s="1">
+        <v>14</v>
+      </c>
+    </row>
   </sheetData>
+  <sheetProtection selectLockedCells="1" selectUnlockedCells="1"/>
   <mergeCells count="6">
     <mergeCell ref="A1:A2"/>
     <mergeCell ref="B1:B2"/>
@@ -724,7 +998,8 @@
     <mergeCell ref="F1:F2"/>
     <mergeCell ref="G1:G2"/>
   </mergeCells>
-  <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
+  <pageMargins left="0.7" right="0.7" top="0.7875" bottom="0.7875" header="0.511805555555556" footer="0.511805555555556"/>
+  <pageSetup horizontalDpi="300" verticalDpi="300" orientation="portrait" paperSize="9"/>
+  <headerFooter alignWithMargins="0"/>
 </worksheet>
 </file>
</xml_diff>